<commit_message>
feat: fim do exp24
</commit_message>
<xml_diff>
--- a/SLMs_Raridade_Aprimorada.xlsx
+++ b/SLMs_Raridade_Aprimorada.xlsx
@@ -1679,7 +1679,11 @@
       <c r="Q17" t="n">
         <v>1.634285714285714</v>
       </c>
-      <c r="R17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2601,7 +2605,11 @@
       <c r="Q30" t="n">
         <v>1.634285714285714</v>
       </c>
-      <c r="R30" t="inlineStr"/>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">

</xml_diff>